<commit_message>
fixes in diagrams, xlsx and sprawko
</commit_message>
<xml_diff>
--- a/Zadanie 1 - Sprawozdanie/Dane.xlsx
+++ b/Zadanie 1 - Sprawozdanie/Dane.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hubertj\Desktop\s\KSR\zadanie\KSR\Zadanie 1 - Sprawozdanie\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="108" windowWidth="22980" windowHeight="9552" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_xltb_storage_" sheetId="3" state="veryHidden" r:id="rId1"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
   <si>
     <t>Places</t>
   </si>
@@ -62,11 +67,164 @@
   <si>
     <t>D:\Nauka\GitHub\KSR\Zadanie 1 - Sprawozdanie\Rysunki\TF-80-60-40-topics.png</t>
   </si>
+  <si>
+    <t>69,5</t>
+  </si>
+  <si>
+    <t>75,3</t>
+  </si>
+  <si>
+    <t>78,3</t>
+  </si>
+  <si>
+    <t>80,7</t>
+  </si>
+  <si>
+    <t>75,1</t>
+  </si>
+  <si>
+    <t>78,2</t>
+  </si>
+  <si>
+    <t>79,3</t>
+  </si>
+  <si>
+    <t>80,5</t>
+  </si>
+  <si>
+    <t>80,3</t>
+  </si>
+  <si>
+    <t>80,4</t>
+  </si>
+  <si>
+    <t>80,6</t>
+  </si>
+  <si>
+    <t>80,8</t>
+  </si>
+  <si>
+    <t>80,9</t>
+  </si>
+  <si>
+    <t>14,9</t>
+  </si>
+  <si>
+    <t>49,3</t>
+  </si>
+  <si>
+    <t>46,3</t>
+  </si>
+  <si>
+    <t>51,5</t>
+  </si>
+  <si>
+    <t>45,5</t>
+  </si>
+  <si>
+    <t>47,8</t>
+  </si>
+  <si>
+    <t>48,5</t>
+  </si>
+  <si>
+    <t>44,8</t>
+  </si>
+  <si>
+    <t>53,7</t>
+  </si>
+  <si>
+    <t>48,8</t>
+  </si>
+  <si>
+    <t>63,4</t>
+  </si>
+  <si>
+    <t>58,5</t>
+  </si>
+  <si>
+    <t>56,1</t>
+  </si>
+  <si>
+    <t>17,1</t>
+  </si>
+  <si>
+    <t>53,2</t>
+  </si>
+  <si>
+    <t>51,6</t>
+  </si>
+  <si>
+    <t>56,5</t>
+  </si>
+  <si>
+    <t>46,8</t>
+  </si>
+  <si>
+    <t>47,6</t>
+  </si>
+  <si>
+    <t>52,4</t>
+  </si>
+  <si>
+    <t>71,4</t>
+  </si>
+  <si>
+    <t>81,1</t>
+  </si>
+  <si>
+    <t>82,6</t>
+  </si>
+  <si>
+    <t>83,1</t>
+  </si>
+  <si>
+    <t>83,5</t>
+  </si>
+  <si>
+    <t>80,2</t>
+  </si>
+  <si>
+    <t>79,4</t>
+  </si>
+  <si>
+    <t>77,3</t>
+  </si>
+  <si>
+    <t>78,5</t>
+  </si>
+  <si>
+    <t>79,2</t>
+  </si>
+  <si>
+    <t>79,6</t>
+  </si>
+  <si>
+    <t>55,2</t>
+  </si>
+  <si>
+    <t>56,7</t>
+  </si>
+  <si>
+    <t>41,3</t>
+  </si>
+  <si>
+    <t>41,8</t>
+  </si>
+  <si>
+    <t>40,8</t>
+  </si>
+  <si>
+    <t>42,3</t>
+  </si>
+  <si>
+    <t>50,7</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,7 +293,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -143,14 +301,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -248,6 +409,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A709-4504-B5E6-F0573B1B77ED}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -299,6 +465,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A709-4504-B5E6-F0573B1B77ED}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -352,6 +523,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A709-4504-B5E6-F0573B1B77ED}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -388,6 +564,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -425,6 +602,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -438,6 +616,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -453,7 +632,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -465,9 +644,9 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -549,6 +728,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A06E-443A-94A9-D7FAAE40F86B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -612,6 +796,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A06E-443A-94A9-D7FAAE40F86B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -678,6 +867,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A06E-443A-94A9-D7FAAE40F86B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -782,7 +976,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -794,9 +988,9 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -878,6 +1072,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EDD1-43A6-9D5F-2232DC6246CF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -941,6 +1140,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EDD1-43A6-9D5F-2232DC6246CF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1007,6 +1211,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-EDD1-43A6-9D5F-2232DC6246CF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1112,7 +1321,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1124,9 +1333,9 @@
 </file>
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1208,6 +1417,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FBD9-40A8-9074-4ACBE42FBBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1271,6 +1485,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBD9-40A8-9074-4ACBE42FBBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1337,6 +1556,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FBD9-40A8-9074-4ACBE42FBBA3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1441,7 +1665,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1453,9 +1677,9 @@
 </file>
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1522,9 +1746,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4056-4505-B2EA-0EDCBEFCDA87}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1573,9 +1814,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4056-4505-B2EA-0EDCBEFCDA87}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1627,9 +1885,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4056-4505-B2EA-0EDCBEFCDA87}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1666,6 +1941,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1703,6 +1979,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1716,6 +1993,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1731,7 +2009,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1743,9 +2021,9 @@
 </file>
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1808,13 +2086,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'WC - Podział Zbiorów - OWN'!$C$14:$C$17</c:f>
+              <c:f>'WC - Podział Zbiorów - OWN'!$C$14:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9890-4457-B642-69267E76F73C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1863,9 +2155,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9890-4457-B642-69267E76F73C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1913,13 +2222,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'WC - Podział Zbiorów - OWN'!$I$14:$I$17</c:f>
+              <c:f>'WC - Podział Zbiorów - OWN'!$I$15:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9890-4457-B642-69267E76F73C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1956,6 +2279,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1993,6 +2317,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2006,6 +2331,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2021,7 +2347,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2033,9 +2359,9 @@
 </file>
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2102,9 +2428,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FC8F-4974-AC65-82E21CA23C7D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2153,9 +2496,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FC8F-4974-AC65-82E21CA23C7D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2207,9 +2567,26 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-FC8F-4974-AC65-82E21CA23C7D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2246,6 +2623,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2283,6 +2661,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2296,6 +2675,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2311,7 +2691,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2323,9 +2703,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2423,6 +2803,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F417-4471-87B4-61874D14A481}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2474,6 +2859,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F417-4471-87B4-61874D14A481}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2527,6 +2917,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F417-4471-87B4-61874D14A481}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2563,6 +2958,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2600,6 +2996,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2613,6 +3010,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2628,7 +3026,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2640,9 +3038,9 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2740,6 +3138,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-36F1-48E6-985E-91614810B01E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2791,6 +3194,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-36F1-48E6-985E-91614810B01E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2844,6 +3252,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-36F1-48E6-985E-91614810B01E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2880,6 +3293,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2917,6 +3331,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2930,6 +3345,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2945,7 +3361,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2957,9 +3373,9 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3057,6 +3473,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A2BB-477A-B19D-F6633B022245}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3108,6 +3529,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A2BB-477A-B19D-F6633B022245}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3161,6 +3587,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A2BB-477A-B19D-F6633B022245}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3265,7 +3696,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3277,9 +3708,9 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3377,6 +3808,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6610-4443-8BFB-9EF65E106F8D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3428,6 +3864,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6610-4443-8BFB-9EF65E106F8D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3481,6 +3922,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6610-4443-8BFB-9EF65E106F8D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3585,7 +4031,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3597,9 +4043,9 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3697,6 +4143,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3596-4059-8686-F4929EA14FB3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3748,6 +4199,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3596-4059-8686-F4929EA14FB3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3801,6 +4257,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3596-4059-8686-F4929EA14FB3}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3905,7 +4366,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3917,9 +4378,9 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3993,8 +4454,14 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>79.400000000000006</c:v>
@@ -4004,10 +4471,18 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F4EB-4A8B-A137-BE03E0247009}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4065,9 +4540,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F4EB-4A8B-A137-BE03E0247009}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4127,9 +4628,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F4EB-4A8B-A137-BE03E0247009}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4234,7 +4761,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4246,9 +4773,9 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4322,9 +4849,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ACB9-4A73-8C7B-6D747BE919E5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4352,9 +4905,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-ACB9-4A73-8C7B-6D747BE919E5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4384,9 +4963,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-ACB9-4A73-8C7B-6D747BE919E5}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4491,7 +5096,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4503,9 +5108,9 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pl-PL"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4579,9 +5184,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8A2C-49D7-85F8-704ED95AADAE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4609,9 +5240,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8A2C-49D7-85F8-704ED95AADAE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4641,9 +5298,35 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8A2C-49D7-85F8-704ED95AADAE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4748,7 +5431,7 @@
           <a:latin typeface="LM Roman 12" pitchFamily="50" charset="-18"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5263,9 +5946,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5303,9 +5986,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5340,7 +6023,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5375,7 +6058,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5585,7 +6268,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="I19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6091,11 +6774,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
     <mergeCell ref="B26:I26"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="E28:F28"/>
@@ -6103,6 +6781,11 @@
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6114,7 +6797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -6620,11 +7303,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B14:I14"/>
     <mergeCell ref="B26:I26"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="E28:F28"/>
@@ -6632,6 +7310,11 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6643,8 +7326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6679,41 +7362,60 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E5">
         <v>2</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>69</v>
+      </c>
       <c r="H5">
         <v>2</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E6">
         <v>3</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="H6">
         <v>3</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>78.3</v>
+      <c r="C7" t="s">
+        <v>13</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="H7">
         <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
@@ -6726,9 +7428,14 @@
       <c r="E8">
         <v>7</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="H8">
         <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -6741,9 +7448,14 @@
       <c r="E9">
         <v>10</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2">
+        <v>80</v>
+      </c>
       <c r="H9">
         <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -6756,22 +7468,34 @@
       <c r="E10">
         <v>15</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H10">
         <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>20</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E11">
         <v>20</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="H11">
         <v>20</v>
+      </c>
+      <c r="I11" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
@@ -6804,91 +7528,140 @@
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H17">
         <v>2</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>3</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>53</v>
+      </c>
       <c r="E18">
         <v>3</v>
       </c>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2">
+        <v>47</v>
+      </c>
       <c r="H18">
         <v>3</v>
+      </c>
+      <c r="I18">
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>5</v>
       </c>
+      <c r="C19">
+        <v>47</v>
+      </c>
       <c r="E19">
         <v>5</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>47</v>
+      </c>
       <c r="H19">
         <v>5</v>
+      </c>
+      <c r="I19">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>7</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E20">
         <v>7</v>
       </c>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="H20">
         <v>7</v>
+      </c>
+      <c r="I20">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>10</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="E21">
         <v>10</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="H21">
         <v>10</v>
+      </c>
+      <c r="I21">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>15</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E22">
         <v>15</v>
       </c>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H22">
         <v>15</v>
+      </c>
+      <c r="I22">
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E23">
         <v>20</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="H23">
         <v>20</v>
+      </c>
+      <c r="I23">
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
@@ -6921,77 +7694,140 @@
       <c r="B29">
         <v>2</v>
       </c>
+      <c r="C29" t="s">
+        <v>31</v>
+      </c>
       <c r="E29">
         <v>2</v>
       </c>
+      <c r="F29" t="s">
+        <v>36</v>
+      </c>
       <c r="H29">
         <v>2</v>
+      </c>
+      <c r="I29" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>3</v>
       </c>
+      <c r="C30" t="s">
+        <v>32</v>
+      </c>
       <c r="E30">
         <v>3</v>
       </c>
+      <c r="F30" t="s">
+        <v>36</v>
+      </c>
       <c r="H30">
         <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>5</v>
       </c>
+      <c r="C31" t="s">
+        <v>33</v>
+      </c>
       <c r="E31">
         <v>5</v>
       </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
       <c r="H31">
         <v>5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32">
         <v>7</v>
       </c>
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
       <c r="E32">
         <v>7</v>
       </c>
+      <c r="F32" t="s">
+        <v>35</v>
+      </c>
       <c r="H32">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33">
         <v>10</v>
       </c>
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
       <c r="E33">
         <v>10</v>
       </c>
+      <c r="F33">
+        <v>61</v>
+      </c>
       <c r="H33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34">
         <v>15</v>
       </c>
+      <c r="C34" t="s">
+        <v>35</v>
+      </c>
       <c r="E34">
         <v>15</v>
       </c>
+      <c r="F34" t="s">
+        <v>35</v>
+      </c>
       <c r="H34">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="I34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35">
         <v>20</v>
       </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
       <c r="E35">
         <v>20</v>
       </c>
+      <c r="F35" t="s">
+        <v>36</v>
+      </c>
       <c r="H35">
         <v>20</v>
+      </c>
+      <c r="I35" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -7018,8 +7854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7367,7 +8203,7 @@
   <dimension ref="B2:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7402,44 +8238,80 @@
       <c r="B5">
         <v>5</v>
       </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
       <c r="E5">
         <v>5</v>
       </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
       <c r="H5">
         <v>5</v>
+      </c>
+      <c r="I5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>7</v>
       </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
       <c r="E6">
         <v>7</v>
       </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
       <c r="H6">
         <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
       <c r="E7">
         <v>10</v>
       </c>
+      <c r="F7" t="s">
+        <v>49</v>
+      </c>
       <c r="H7">
         <v>10</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>15</v>
       </c>
+      <c r="C8" t="s">
+        <v>48</v>
+      </c>
       <c r="E8">
         <v>15</v>
       </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
       <c r="H8">
         <v>15</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
@@ -7472,48 +8344,80 @@
       <c r="B14">
         <v>7</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E14">
         <v>7</v>
       </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
       <c r="H14">
         <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>10</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="E15">
         <v>10</v>
       </c>
+      <c r="F15" t="s">
+        <v>25</v>
+      </c>
       <c r="H15">
         <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E16">
         <v>15</v>
       </c>
+      <c r="F16" t="s">
+        <v>29</v>
+      </c>
       <c r="H16">
         <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>20</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="E17">
         <v>20</v>
       </c>
+      <c r="F17" t="s">
+        <v>31</v>
+      </c>
       <c r="H17">
         <v>20</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
@@ -7546,45 +8450,80 @@
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
       <c r="E23">
         <v>2</v>
       </c>
+      <c r="F23" t="s">
+        <v>36</v>
+      </c>
       <c r="H23">
         <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>3</v>
       </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
       <c r="E24">
         <v>3</v>
       </c>
+      <c r="F24" t="s">
+        <v>32</v>
+      </c>
       <c r="H24">
         <v>3</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>5</v>
       </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
       <c r="E25">
         <v>5</v>
       </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
       <c r="H25">
         <v>5</v>
+      </c>
+      <c r="I25" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>7</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="E26">
         <v>7</v>
       </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
       <c r="H26">
         <v>7</v>
+      </c>
+      <c r="I26" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>